<commit_message>
Initial improvements for breakdowns
</commit_message>
<xml_diff>
--- a/i2b2/brisskit/trunk/i2b2-uploader/src/test/resources/spreadsheets/EG1-laheart.xlsx
+++ b/i2b2/brisskit/trunk/i2b2-uploader/src/test/resources/spreadsheets/EG1-laheart.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="502" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="502" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="LAHEART" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="LOOKUP" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="BREAKDOWNS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="LAHEART" vbProcedure="false">LAHEART!$A$1:$R$203</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>ID</t>
   </si>
@@ -221,6 +222,18 @@
   <si>
     <t>Dead</t>
   </si>
+  <si>
+    <t>breakdown</t>
+  </si>
+  <si>
+    <t>column heading</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Vital Status</t>
+  </si>
 </sst>
 </file>
 
@@ -229,7 +242,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="MS Sans Serif"/>
       <charset val="1"/>
@@ -249,6 +262,11 @@
     <font>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -300,7 +318,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
@@ -308,6 +326,7 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -327,28 +346,29 @@
   </sheetPr>
   <dimension ref="A1:R203"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="F177" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="J207" activeCellId="0" pane="topLeft" sqref="J207"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4274509803922"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.721568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9019607843137"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6549019607843"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8039215686275"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3803921568627"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4392156862745"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.7843137254902"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3607843137255"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.7294117647059"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.4352941176471"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.7098039215686"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.3490196078431"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7686274509804"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9490196078431"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7176470588235"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.7529411764706"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.9019607843137"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.443137254902"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.5098039215686"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.843137254902"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.4235294117647"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.8627450980392"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.7843137254902"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.4901960784314"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.7647058823529"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.4039215686275"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.52941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1" s="2">
@@ -11737,15 +11757,15 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.443137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.28627450980392"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.5921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.30980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -11858,7 +11878,7 @@
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.25" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.25" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>17</v>
       </c>
@@ -11869,7 +11889,7 @@
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.25" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.25" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>17</v>
       </c>
@@ -11889,4 +11909,55 @@
     <oddFooter>&amp;C&amp;"Arial,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100">
+      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9411764705882"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9803921568627"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.25" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.25" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.25" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>